<commit_message>
test data for integration tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaProjects\swift-rest-api\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807BF6BB-BCDE-47C1-ACFA-DEFE2530CA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E298AD3A-2806-44B5-98CF-EF84F90E1DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>COUNTRY ISO2 CODE</t>
   </si>
@@ -47,43 +47,10 @@
     <t>TIME ZONE</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>AAISALTRXXX</t>
-  </si>
-  <si>
     <t>BIC11</t>
   </si>
   <si>
-    <t>UNITED BANK OF ALBANIA SH.A</t>
-  </si>
-  <si>
-    <t>HYRJA 3 RR. DRITAN HOXHA ND. 11 TIRANA, TIRANA, 1023</t>
-  </si>
-  <si>
-    <t>TIRANA</t>
-  </si>
-  <si>
-    <t>ALBANIA</t>
-  </si>
-  <si>
-    <t>Europe/Tirane</t>
-  </si>
-  <si>
     <t>BG</t>
-  </si>
-  <si>
-    <t>ABIEBGS1XXX</t>
-  </si>
-  <si>
-    <t>ABV INVESTMENTS LTD</t>
-  </si>
-  <si>
-    <t>TSAR ASEN 20  VARNA, VARNA, 9002</t>
-  </si>
-  <si>
-    <t>VARNA</t>
   </si>
   <si>
     <t>BULGARIA</t>
@@ -123,6 +90,111 @@
   </si>
   <si>
     <t>America/Montevideo</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>BIGBPLPWCUS</t>
+  </si>
+  <si>
+    <t>BANK MILLENNIUM S.A.</t>
+  </si>
+  <si>
+    <t>HARMONY CENTER UL. STANISLAWA ZARYNA 2A WARSZAWA, MAZOWIECKIE, 02-593</t>
+  </si>
+  <si>
+    <t>WARSZAWA</t>
+  </si>
+  <si>
+    <t>POLAND</t>
+  </si>
+  <si>
+    <t>Europe/Warsaw</t>
+  </si>
+  <si>
+    <t>BIGBPLPWXXX</t>
+  </si>
+  <si>
+    <t>BISPPLP1XXX</t>
+  </si>
+  <si>
+    <t>BANK INICJATYW SPOLECZNO-EKONOMICZNYCH S.A.</t>
+  </si>
+  <si>
+    <t>DUBOIS STREET 5 A  WARSZAWA, MAZOWIECKIE, 00-184</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>BJSBMCMXLCO</t>
+  </si>
+  <si>
+    <t>BANQUE J. SAFRA SARASIN (MONACO) SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  MONACO, MONACO, 98000</t>
+  </si>
+  <si>
+    <t>MONACO</t>
+  </si>
+  <si>
+    <t>Europe/Monaco</t>
+  </si>
+  <si>
+    <t>BJSBMCMXXXX</t>
+  </si>
+  <si>
+    <t>LE BELLE EPOQUE 15BIS/17 AVENUE D'OSTENDE MONACO, MONACO, 98000</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>BKSACLRM055</t>
+  </si>
+  <si>
+    <t>SCOTIABANK CHILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>SANTIAGO</t>
+  </si>
+  <si>
+    <t>CHILE</t>
+  </si>
+  <si>
+    <t>Pacific/Easter</t>
+  </si>
+  <si>
+    <t>BKSACLRM061</t>
+  </si>
+  <si>
+    <t>VALPARAISO</t>
+  </si>
+  <si>
+    <t>BKSACLRM064</t>
+  </si>
+  <si>
+    <t>21 DE MAYO 187  ARICA, PROVINCIA DE ARICA, 1000000</t>
+  </si>
+  <si>
+    <t>ARICA</t>
+  </si>
+  <si>
+    <t>BKSACLRM068</t>
+  </si>
+  <si>
+    <t>CONCEPCION</t>
+  </si>
+  <si>
+    <t>BKSACLRMXXX</t>
+  </si>
+  <si>
+    <t>AVENIDA COSTANERA SUR 2710, FLOOR 10 EDIFICIO PARQUE TITANIUM SANTIAGO, PROVINCIA DE SANTIAGO</t>
   </si>
 </sst>
 </file>
@@ -168,11 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -394,7 +467,7 @@
   <dimension ref="A1:K1062"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -439,163 +512,291 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
+      <c r="A3" s="4" t="s">
+        <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
+      <c r="B3" s="4" t="s">
+        <v>30</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
+      <c r="H3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -14316,54 +14517,54 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>